<commit_message>
Add cloud price estimations
</commit_message>
<xml_diff>
--- a/logs/Google-Azure-estimation.xlsx
+++ b/logs/Google-Azure-estimation.xlsx
@@ -184,12 +184,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -262,7 +268,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -278,11 +284,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -302,15 +308,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -338,7 +344,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -402,7 +408,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -414,7 +420,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>

</xml_diff>